<commit_message>
fixed units in Table S2
</commit_message>
<xml_diff>
--- a/tables/TableS2_COSIMO_nutrient_key.xlsx
+++ b/tables/TableS2_COSIMO_nutrient_key.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/Health-Benefit-Calculation-BFA/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6784C21E-FC77-8749-BA9A-7D1287DB098D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9AB858D-5993-EC42-AB94-8E0B9630EFFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16220" yWindow="5380" windowWidth="21780" windowHeight="14180"/>
+    <workbookView xWindow="16220" yWindow="5380" windowWidth="21780" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COSIMO_nutrient_key" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,15 @@
     <t>Calcium</t>
   </si>
   <si>
-    <t>mg/p/d</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
-    <t>Kcal/p/d</t>
-  </si>
-  <si>
     <t>Iron</t>
   </si>
   <si>
     <t>Monounsaturated fatty acids</t>
   </si>
   <si>
-    <t>g/p/d</t>
-  </si>
-  <si>
     <t>Omega-3 fatty acids</t>
   </si>
   <si>
@@ -61,21 +52,12 @@
     <t>Vitamin A, RAE</t>
   </si>
   <si>
-    <t>mg/p/d retinol</t>
-  </si>
-  <si>
     <t>Vitamin A</t>
   </si>
   <si>
-    <t>IU/p/d</t>
-  </si>
-  <si>
     <t>Vitamin B-12</t>
   </si>
   <si>
-    <t>ug/p/d</t>
-  </si>
-  <si>
     <t>Zinc</t>
   </si>
   <si>
@@ -98,12 +80,30 @@
   </si>
   <si>
     <t>Macronutrient</t>
+  </si>
+  <si>
+    <t>g/d</t>
+  </si>
+  <si>
+    <t>Kcal/d</t>
+  </si>
+  <si>
+    <t>mg/d</t>
+  </si>
+  <si>
+    <t>IU/d</t>
+  </si>
+  <si>
+    <t>mg/d retinol</t>
+  </si>
+  <si>
+    <t>ug/d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -947,11 +947,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -963,156 +963,156 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>